<commit_message>
Fixed label title in excel file
</commit_message>
<xml_diff>
--- a/Project/static/download_example/implied_distribution_market_application_dataset.xlsx
+++ b/Project/static/download_example/implied_distribution_market_application_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Flask_London\Project\static\download_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00ADDDE-B198-4F5B-806E-CDAAA43957D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5A8B4-1232-415C-B847-1D19C48F232A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98C8B20F-991F-4BF6-ADCD-80D53DFB5FF1}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>Put_Price</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Deselect Line</t>
   </si>
   <si>
     <t>Strike</t>
+  </si>
+  <si>
+    <t>Time to Maturity</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,12 +421,12 @@
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -435,10 +435,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified style of file excel enabled file excel to temp and pca model
</commit_message>
<xml_diff>
--- a/Project/static/download_example/implied_distribution_market_application_dataset.xlsx
+++ b/Project/static/download_example/implied_distribution_market_application_dataset.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Flask_London\Project\static\download_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Workspace\Flask_London\Project\static\download_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5A8B4-1232-415C-B847-1D19C48F232A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98C8B20F-991F-4BF6-ADCD-80D53DFB5FF1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="data_shimko_market" sheetId="1" r:id="rId1"/>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,10 +90,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -408,23 +412,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E463EDD-C1A3-4223-82C6-F5542086180C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -441,178 +445,189 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>325</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>66.5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>0.3125</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
         <f>2/12</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>345</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>46</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.875</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>360</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>365</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>27.75</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>2.625</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>375</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>20.175000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>4.25</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>385</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>13.5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>7.125</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>390</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>9.625</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>8.75</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>0</v>
       </c>
+      <c r="E8" s="3"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>395</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>7.25</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>11</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>400</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>5.375</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>13.75</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>405</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>3.375</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>17</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>410</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>1.875</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>19.75</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>425</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>0.25</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>34</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>